<commit_message>
Se implementan cambio versión 1.2.2 II
</commit_message>
<xml_diff>
--- a/public/plantillas/plantilla_bateria_pruebas.xlsx
+++ b/public/plantillas/plantilla_bateria_pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abort\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CB9475-C886-48A0-8E0E-F81C5638E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA01D09-90EB-45D8-BE16-82E8A505E041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8A47BA8A-C8E5-4D6E-8247-3AAD37052700}"/>
+    <workbookView xWindow="28680" yWindow="960" windowWidth="25440" windowHeight="15390" xr2:uid="{8A47BA8A-C8E5-4D6E-8247-3AAD37052700}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>REG-AUV-0471</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>ko</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>ID Prueba</t>
@@ -65,6 +62,12 @@
   </si>
   <si>
     <t>❌ El sistema no procesó correctamente la eliminación del servicio con retirada, generando un error inesperado.</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>18.1.X</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -164,11 +167,54 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -519,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8C84E3-05B3-40A4-BD01-99A82B943F30}">
-  <dimension ref="A2:F7"/>
+  <dimension ref="A2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,29 +578,33 @@
     <col min="3" max="3" width="45.28515625" customWidth="1"/>
     <col min="4" max="4" width="52.85546875" customWidth="1"/>
     <col min="5" max="5" width="66.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -562,60 +612,75 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D7">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
     <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
@@ -623,7 +688,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F7">
+  <conditionalFormatting sqref="F3">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"KO"</formula>
     </cfRule>

</xml_diff>